<commit_message>
Add `meas_remove_neg_values` option so that we can choose whether to clip the negative values or subtract the minimum; Refine `load_raw` by adding a file size check; Update `params/paper` and paper related notebooks
</commit_message>
<xml_diff>
--- a/docs/20241219_GPU_comparison/GPU_comparison.xlsx
+++ b/docs/20241219_GPU_comparison/GPU_comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\workspace\ptyrad\docs\20241219_GPU_comparison\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chiahao3\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E797AE03-85F5-42D6-B652-CAD2C55A3FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32ACA3F8-69C4-46FF-B5C6-606CCB1BDEB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{BCE30958-3EF4-41C1-A9CA-400A59448C92}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BCE30958-3EF4-41C1-A9CA-400A59448C92}"/>
   </bookViews>
   <sheets>
     <sheet name="Throughput" sheetId="2" r:id="rId1"/>
@@ -93,8 +93,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -139,19 +140,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -169,7 +172,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-TW"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -277,7 +280,6 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
-            <c:intercept val="0"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -321,7 +323,7 @@
             <c:numRef>
               <c:f>Throughput!$B$2:$B$8</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.28849999999999998</c:v>
@@ -330,19 +332,19 @@
                   <c:v>0.44800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.76800000000000002</c:v>
+                  <c:v>0.57599999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.76800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.01</c:v>
+                  <c:v>0.76800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.57599999999999996</c:v>
+                  <c:v>0.96</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.96</c:v>
+                  <c:v>1.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -351,7 +353,7 @@
             <c:numRef>
               <c:f>Throughput!$E$2:$E$8</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>9.1249201569486266E-2</c:v>
@@ -360,19 +362,19 @@
                   <c:v>0.15266010228226851</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.23135295206366832</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.27588490081937816</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.26602819898909286</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.38128646051778703</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.23135295206366832</c:v>
+                  <c:v>0.35660794522501965</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.35660794522501965</c:v>
+                  <c:v>0.38128646051778703</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -471,7 +473,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -588,7 +590,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -685,7 +687,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-TW"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -845,20 +847,20 @@
                 <c:pt idx="1">
                   <c:v>19.170000000000002</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="2" formatCode="General">
+                  <c:v>65.28</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>27.77</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>38.71</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>82.58</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>65.28</c:v>
+                <c:pt idx="5">
+                  <c:v>91.06</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>91.06</c:v>
+                  <c:v>82.58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -867,7 +869,7 @@
             <c:numRef>
               <c:f>Throughput!$E$2:$E$8</c:f>
               <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
+                <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>9.1249201569486266E-2</c:v>
@@ -876,19 +878,19 @@
                   <c:v>0.15266010228226851</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.23135295206366832</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.27588490081937816</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>0.26602819898909286</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.38128646051778703</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.23135295206366832</c:v>
+                  <c:v>0.35660794522501965</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.35660794522501965</c:v>
+                  <c:v>0.38128646051778703</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1104,7 +1106,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2321,7 +2323,7 @@
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>427167</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>116541</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2351,13 +2353,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>152401</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>8964</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>457201</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>125506</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2389,7 +2391,7 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>206188</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>107576</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="545214" cy="264560"/>
@@ -2447,7 +2449,7 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>107576</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>107577</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="545983" cy="264560"/>
@@ -2506,7 +2508,7 @@
       <xdr:col>11</xdr:col>
       <xdr:colOff>340659</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>71717</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="713593" cy="264560"/>
     <xdr:sp macro="" textlink="">
@@ -2564,7 +2566,7 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>430306</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>107577</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="545983" cy="264560"/>
     <xdr:sp macro="" textlink="">
@@ -2766,7 +2768,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3084,19 +3086,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8C90F66-59E1-46D4-97E9-724B95343CFB}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="4" width="12.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
+    <col min="3" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>9</v>
       </c>
@@ -3113,146 +3115,146 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="8">
         <v>0.28849999999999998</v>
       </c>
       <c r="C2" s="1">
         <v>8.8729999999999993</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="10">
         <v>10.959</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="10">
         <f>1/D2</f>
         <v>9.1249201569486266E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="8">
         <v>0.44800000000000001</v>
       </c>
       <c r="C3" s="1">
         <v>19.170000000000002</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="10">
         <v>6.5505000000000004</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="10">
         <f t="shared" ref="E3:E14" si="0">1/D3</f>
         <v>0.15266010228226851</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="9">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="C4">
+        <v>65.28</v>
+      </c>
+      <c r="D4" s="9">
+        <v>4.3224</v>
+      </c>
+      <c r="E4" s="10">
+        <f>1/D4</f>
+        <v>0.23135295206366832</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B5" s="8">
         <v>0.76800000000000002</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C5" s="1">
         <v>27.77</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D5" s="10">
         <v>3.6246999999999998</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E5" s="10">
         <f t="shared" si="0"/>
         <v>0.27588490081937816</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B6" s="8">
         <v>0.76800000000000002</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C6" s="1">
         <v>38.71</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D6" s="10">
         <v>3.7589999999999999</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E6" s="10">
         <f t="shared" si="0"/>
         <v>0.26602819898909286</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0.96</v>
+      </c>
+      <c r="C7" s="1">
+        <v>91.06</v>
+      </c>
+      <c r="D7" s="10">
+        <v>2.8041999999999998</v>
+      </c>
+      <c r="E7" s="10">
+        <f>1/D7</f>
+        <v>0.35660794522501965</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
         <v>4090</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B8" s="8">
         <v>1.01</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C8" s="1">
         <v>82.58</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D8" s="10">
         <v>2.6227</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E8" s="10">
         <f t="shared" si="0"/>
         <v>0.38128646051778703</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="3">
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="C7">
-        <v>65.28</v>
-      </c>
-      <c r="D7" s="3">
-        <v>4.3224</v>
-      </c>
-      <c r="E7" s="7">
-        <f>1/D7</f>
-        <v>0.23135295206366832</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="3">
-        <v>0.96</v>
-      </c>
-      <c r="C8" s="1">
-        <v>91.06</v>
-      </c>
-      <c r="D8" s="7">
-        <v>2.8041999999999998</v>
-      </c>
-      <c r="E8" s="7">
-        <f>1/D8</f>
-        <v>0.35660794522501965</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>2.04</v>
       </c>
       <c r="C9" s="1">
         <v>19.489999999999998</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>1.79</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <f>1/D9</f>
         <v>0.55865921787709494</v>
       </c>
@@ -3260,18 +3262,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <f>B13/7</f>
         <v>0.29142857142857143</v>
       </c>
@@ -3279,19 +3281,19 @@
         <f>C13/7</f>
         <v>2.7842857142857143</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>12.464</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <f t="shared" si="0"/>
         <v>8.0231065468549426E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <f>B13*2/7</f>
         <v>0.58285714285714285</v>
       </c>
@@ -3299,66 +3301,66 @@
         <f>C13*2/7</f>
         <v>5.5685714285714285</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="6">
         <v>6.4671000000000003</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <f t="shared" si="0"/>
         <v>0.15462881353311375</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>2.04</v>
       </c>
       <c r="C13" s="1">
         <v>19.489999999999998</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>1.8869</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="6">
         <f t="shared" si="0"/>
         <v>0.52996979172187186</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>3.9380000000000002</v>
       </c>
       <c r="C14" s="1">
         <v>60</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14" s="6">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <f t="shared" si="0"/>
         <v>0.90909090909090906</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
       <c r="E19" s="2"/>
     </row>
   </sheetData>

</xml_diff>